<commit_message>
chainsql results and test scripts
</commit_message>
<xml_diff>
--- a/chainsql_test_results/data/chainsql_test_results.xlsx
+++ b/chainsql_test_results/data/chainsql_test_results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgedinicola/Desktop/comse6156-experiment/chainsql_test_results/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05469CB6-AB8F-F24C-A639-08FC8A74F02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17309291-46FC-7A4B-A53C-51DD9F98371C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29740" yWindow="3040" windowWidth="28040" windowHeight="17440" xr2:uid="{3F5778E9-4CED-B04E-BAD7-E48EF596859C}"/>
+    <workbookView xWindow="68800" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{3F5778E9-4CED-B04E-BAD7-E48EF596859C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C8409F-410B-164A-B6EA-48CA3B22951B}">
   <dimension ref="C2:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,10 +470,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>6</v>
@@ -487,31 +487,31 @@
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="D4" s="3">
-        <f>AVERAGE(D5:D104)</f>
+        <f t="shared" ref="D4:J4" si="0">AVERAGE(D5:D104)</f>
         <v>1.0287900000000012</v>
       </c>
       <c r="E4" s="3">
-        <f>AVERAGE(E5:E104)</f>
+        <f t="shared" si="0"/>
         <v>4.5409999999999992E-2</v>
       </c>
       <c r="F4" s="3">
         <f>AVERAGE(F5:F104)</f>
-        <v>2.3739999999999973E-2</v>
+        <v>3.2659999999999981E-2</v>
       </c>
       <c r="G4" s="3">
         <f>AVERAGE(G5:G104)</f>
-        <v>3.2659999999999981E-2</v>
+        <v>2.3739999999999973E-2</v>
       </c>
       <c r="H4" s="3">
-        <f>AVERAGE(H5:H104)</f>
+        <f t="shared" si="0"/>
         <v>2.4079999999999994E-2</v>
       </c>
       <c r="I4" s="3">
-        <f>AVERAGE(I5:I104)</f>
+        <f t="shared" si="0"/>
         <v>2.4310000000000012E-2</v>
       </c>
       <c r="J4" s="3">
-        <f>AVERAGE(J5:J104)</f>
+        <f t="shared" si="0"/>
         <v>1.9119999999999974E-2</v>
       </c>
     </row>
@@ -569,10 +569,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F7">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G7">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H7">
         <v>2.1000000000000001E-2</v>
@@ -592,10 +592,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F8">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G8">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H8">
         <v>2.1000000000000001E-2</v>
@@ -615,10 +615,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F9">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G9">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H9">
         <v>2.1000000000000001E-2</v>
@@ -638,10 +638,10 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F10">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G10">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H10">
         <v>2.1999999999999999E-2</v>
@@ -661,10 +661,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G11">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H11">
         <v>2.1000000000000001E-2</v>
@@ -684,10 +684,10 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F12">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G12">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H12">
         <v>2.1999999999999999E-2</v>
@@ -753,10 +753,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F15">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G15">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H15">
         <v>2.1999999999999999E-2</v>
@@ -776,10 +776,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F16">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G16">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H16">
         <v>2.1999999999999999E-2</v>
@@ -845,10 +845,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F19">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G19">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H19">
         <v>2.7E-2</v>
@@ -937,10 +937,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F23">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G23">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H23">
         <v>2.1999999999999999E-2</v>
@@ -960,10 +960,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F24">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G24">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H24">
         <v>2.1999999999999999E-2</v>
@@ -983,10 +983,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F25">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G25">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H25">
         <v>2.1000000000000001E-2</v>
@@ -1006,10 +1006,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G26">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G26">
-        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H26">
         <v>2.1999999999999999E-2</v>
@@ -1029,10 +1029,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F27">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G27">
         <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G27">
-        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H27">
         <v>2.1999999999999999E-2</v>
@@ -1052,10 +1052,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F28">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G28">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H28">
         <v>2.1999999999999999E-2</v>
@@ -1075,10 +1075,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F29">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G29">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H29">
         <v>2.1000000000000001E-2</v>
@@ -1098,10 +1098,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F30">
-        <v>2.1999999999999999E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G30">
-        <v>8.5000000000000006E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H30">
         <v>2.5000000000000001E-2</v>
@@ -1121,10 +1121,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F31">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G31">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H31">
         <v>5.0999999999999997E-2</v>
@@ -1144,10 +1144,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F32">
-        <v>0.02</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G32">
-        <v>2.3E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H32">
         <v>3.2000000000000001E-2</v>
@@ -1167,10 +1167,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F33">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G33">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H33">
         <v>0.02</v>
@@ -1213,10 +1213,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F35">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G35">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H35">
         <v>2.1999999999999999E-2</v>
@@ -1236,10 +1236,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F36">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G36">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H36">
         <v>2.1999999999999999E-2</v>
@@ -1282,10 +1282,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F38">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G38">
         <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="G38">
-        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H38">
         <v>2.1999999999999999E-2</v>
@@ -1305,10 +1305,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F39">
-        <v>2.1999999999999999E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G39">
-        <v>2.4E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H39">
         <v>2.1999999999999999E-2</v>
@@ -1328,10 +1328,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F40">
-        <v>2.3E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G40">
-        <v>2.1000000000000001E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H40">
         <v>2.1999999999999999E-2</v>
@@ -1374,10 +1374,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F42">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G42">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H42">
         <v>2.1999999999999999E-2</v>
@@ -1420,10 +1420,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F44">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G44">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H44">
         <v>2.1999999999999999E-2</v>
@@ -1443,10 +1443,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F45">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G45">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H45">
         <v>8.2000000000000003E-2</v>
@@ -1466,10 +1466,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F46">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G46">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H46">
         <v>0.03</v>
@@ -1535,10 +1535,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F49">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G49">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H49">
         <v>2.1999999999999999E-2</v>
@@ -1558,10 +1558,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F50">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G50">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H50">
         <v>2.1999999999999999E-2</v>
@@ -1581,10 +1581,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F51">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G51">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H51">
         <v>2.1999999999999999E-2</v>
@@ -1627,10 +1627,10 @@
         <v>2.4E-2</v>
       </c>
       <c r="F53">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G53">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H53">
         <v>2.1999999999999999E-2</v>
@@ -1673,10 +1673,10 @@
         <v>0.03</v>
       </c>
       <c r="F55">
+        <v>0.02</v>
+      </c>
+      <c r="G55">
         <v>2.7E-2</v>
-      </c>
-      <c r="G55">
-        <v>0.02</v>
       </c>
       <c r="H55">
         <v>2.1999999999999999E-2</v>
@@ -1696,10 +1696,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F56">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G56">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G56">
-        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H56">
         <v>2.1999999999999999E-2</v>
@@ -1719,10 +1719,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F57">
+        <v>0.02</v>
+      </c>
+      <c r="G57">
         <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="G57">
-        <v>0.02</v>
       </c>
       <c r="H57">
         <v>2.1999999999999999E-2</v>
@@ -1742,10 +1742,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F58">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G58">
         <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="G58">
-        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H58">
         <v>2.1999999999999999E-2</v>
@@ -1765,10 +1765,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F59">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G59">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H59">
         <v>2.1999999999999999E-2</v>
@@ -1811,10 +1811,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F61">
-        <v>1.9E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G61">
-        <v>2.1000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H61">
         <v>2.1999999999999999E-2</v>
@@ -1834,10 +1834,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F62">
-        <v>1.9E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G62">
-        <v>2.1000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H62">
         <v>2.1999999999999999E-2</v>
@@ -1857,10 +1857,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F63">
-        <v>2.4E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G63">
-        <v>2.1999999999999999E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H63">
         <v>2.1999999999999999E-2</v>
@@ -1880,10 +1880,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F64">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G64">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H64">
         <v>2.1999999999999999E-2</v>
@@ -1972,10 +1972,10 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F68">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G68">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H68">
         <v>2.1999999999999999E-2</v>
@@ -1995,10 +1995,10 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F69">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G69">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H69">
         <v>2.1999999999999999E-2</v>
@@ -2018,10 +2018,10 @@
         <v>0.06</v>
       </c>
       <c r="F70">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G70">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H70">
         <v>2.1999999999999999E-2</v>
@@ -2041,10 +2041,10 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F71">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G71">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H71">
         <v>2.1999999999999999E-2</v>
@@ -2133,10 +2133,10 @@
         <v>0.11</v>
       </c>
       <c r="F75">
-        <v>2.1999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G75">
-        <v>0.05</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H75">
         <v>2.1000000000000001E-2</v>
@@ -2156,10 +2156,10 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="F76">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G76">
         <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="G76">
-        <v>8.8999999999999996E-2</v>
       </c>
       <c r="H76">
         <v>2.1999999999999999E-2</v>
@@ -2179,10 +2179,10 @@
         <v>0.08</v>
       </c>
       <c r="F77">
-        <v>2.1999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G77">
-        <v>0.03</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H77">
         <v>2.3E-2</v>
@@ -2202,10 +2202,10 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F78">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G78">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H78">
         <v>2.1999999999999999E-2</v>
@@ -2225,10 +2225,10 @@
         <v>6.3E-2</v>
       </c>
       <c r="F79">
-        <v>2.1999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="G79">
-        <v>2.3E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H79">
         <v>2.1999999999999999E-2</v>
@@ -2248,10 +2248,10 @@
         <v>9.4E-2</v>
       </c>
       <c r="F80">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G80">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H80">
         <v>2.3E-2</v>
@@ -2271,10 +2271,10 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="F81">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G81">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H81">
         <v>2.1999999999999999E-2</v>
@@ -2409,10 +2409,10 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F87">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G87">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H87">
         <v>2.3E-2</v>
@@ -2524,10 +2524,10 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F92">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G92">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H92">
         <v>2.1999999999999999E-2</v>
@@ -2593,10 +2593,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F95">
+        <v>0.02</v>
+      </c>
+      <c r="G95">
         <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="G95">
-        <v>0.02</v>
       </c>
       <c r="H95">
         <v>7.1999999999999995E-2</v>
@@ -2616,10 +2616,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F96">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G96">
         <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="G96">
-        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H96">
         <v>2.3E-2</v>
@@ -2639,10 +2639,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F97">
-        <v>2.1999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G97">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H97">
         <v>2.1000000000000001E-2</v>
@@ -2662,10 +2662,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F98">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G98">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H98">
         <v>2.4E-2</v>
@@ -2685,10 +2685,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F99">
-        <v>1.9E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G99">
-        <v>2.1000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H99">
         <v>2.3E-2</v>
@@ -2708,10 +2708,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F100">
-        <v>2.3E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G100">
-        <v>0.02</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H100">
         <v>2.3E-2</v>
@@ -2731,10 +2731,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="F101">
-        <v>2.1000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G101">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H101">
         <v>2.1999999999999999E-2</v>
@@ -2754,10 +2754,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F102">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G102">
-        <v>2.1000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H102">
         <v>2.1999999999999999E-2</v>
@@ -2800,10 +2800,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F104">
-        <v>2.1999999999999999E-2</v>
+        <v>1.0209999999999999</v>
       </c>
       <c r="G104">
-        <v>1.0209999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H104">
         <v>2.1999999999999999E-2</v>

</xml_diff>